<commit_message>
More work, intro, related work, results plots
</commit_message>
<xml_diff>
--- a/2017-AC/serialization.xlsx
+++ b/2017-AC/serialization.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="cpp-serializers" sheetId="1" r:id="rId1"/>
+    <sheet name="osu-daint" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="26">
   <si>
     <t>=</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>ser</t>
+  </si>
+  <si>
+    <t>MB/s</t>
+  </si>
+  <si>
+    <t>rma</t>
+  </si>
+  <si>
+    <t>rma vector</t>
+  </si>
+  <si>
+    <t>serialize buffer</t>
+  </si>
+  <si>
+    <t>Msg Size</t>
+  </si>
+  <si>
+    <t>2 threads</t>
   </si>
 </sst>
 </file>
@@ -164,7 +185,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'cpp-serializers'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -176,7 +197,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>'cpp-serializers'!$A$2:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
@@ -223,7 +244,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:f>'cpp-serializers'!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -279,11 +300,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151599104"/>
-        <c:axId val="198601536"/>
+        <c:axId val="661872128"/>
+        <c:axId val="216547904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151599104"/>
+        <c:axId val="661872128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -292,7 +313,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198601536"/>
+        <c:crossAx val="216547904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -300,7 +321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198601536"/>
+        <c:axId val="216547904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,7 +342,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151599104"/>
+        <c:crossAx val="661872128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -378,7 +399,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>'cpp-serializers'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -390,7 +411,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>'cpp-serializers'!$A$2:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
@@ -437,7 +458,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$14</c:f>
+              <c:f>'cpp-serializers'!$H$2:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -493,11 +514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132746752"/>
-        <c:axId val="198599808"/>
+        <c:axId val="662266368"/>
+        <c:axId val="216549632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132746752"/>
+        <c:axId val="662266368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198599808"/>
+        <c:crossAx val="216549632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -514,7 +535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198599808"/>
+        <c:axId val="216549632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132746752"/>
+        <c:crossAx val="662266368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -544,6 +565,510 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'osu-daint'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>serialize buffer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="4"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'osu-daint'!$A$3:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4194304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'osu-daint'!$E$3:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>3.4179687499999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1884765625000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.65419921875E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3328124999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6730468749999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.321552734375E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.654716796875E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.321220703125E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10555634765624999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.20723544921875001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.38705947265625001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.73152646484374995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.49890498046874998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0598195312500001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0446295898437499</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.8644322265625002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.7420729492187501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.236664453125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.40108134765625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.44327451171875</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.47737197265625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.247168847656249</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.20408125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'osu-daint'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rma vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="4"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'osu-daint'!$A$3:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4194304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'osu-daint'!$J$3:$J$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>3.3164062500000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2939453125000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6734375E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3310546875E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5965820312500001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.33123046875E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6712109375000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3670312499999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10551357421875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21078359375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3891400390625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.72369853515625004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.63301484374999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4063630859375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.7902811523437498</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.6079516601562496</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.08476279296875</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.253412109375001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.4234845703125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.39495302734375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.2620578125</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.5864115234375</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.24517890625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="205936832"/>
+        <c:axId val="205936256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="205936832"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Message size (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="205936256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="205936256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bandwidth GB/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="205936832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21320097364067114"/>
+          <c:y val="7.7353054841745608E-2"/>
+          <c:w val="0.4171583425717994"/>
+          <c:h val="0.2194205592234203"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="800">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -609,6 +1134,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -906,7 +1466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
@@ -1273,13 +1833,887 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="11" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2.8570000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.35</v>
+      </c>
+      <c r="E3">
+        <f>D3/1024</f>
+        <v>3.4179687499999998E-4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>2.9449999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.33960000000000001</v>
+      </c>
+      <c r="J3">
+        <f>I3/1024</f>
+        <v>3.3164062500000001E-4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>2.3853</v>
+      </c>
+      <c r="D4">
+        <v>0.83850000000000002</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E25" si="0">D4/1024</f>
+        <v>8.1884765625000002E-4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>2.3548</v>
+      </c>
+      <c r="I4">
+        <v>0.84930000000000005</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J25" si="1">I4/1024</f>
+        <v>8.2939453125000005E-4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>2.3614999999999999</v>
+      </c>
+      <c r="D5">
+        <v>1.6939</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.65419921875E-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>2.3342999999999998</v>
+      </c>
+      <c r="I5">
+        <v>1.7136</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>1.6734375E-3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>2.3441000000000001</v>
+      </c>
+      <c r="D6">
+        <v>3.4127999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3.3328124999999998E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <v>2.3454000000000002</v>
+      </c>
+      <c r="I6">
+        <v>3.411</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>3.3310546875E-3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>2.3414999999999999</v>
+      </c>
+      <c r="D7">
+        <v>6.8331999999999997</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>6.6730468749999997E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>2.3687</v>
+      </c>
+      <c r="I7">
+        <v>6.7549000000000001</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>6.5965820312500001E-3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>2.3645999999999998</v>
+      </c>
+      <c r="D8">
+        <v>13.5327</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.321552734375E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <v>2.3473999999999999</v>
+      </c>
+      <c r="I8">
+        <v>13.6318</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.33123046875E-2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>2.3542999999999998</v>
+      </c>
+      <c r="D9">
+        <v>27.1843</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.654716796875E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9">
+        <v>2.3397999999999999</v>
+      </c>
+      <c r="I9">
+        <v>27.353200000000001</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>2.6712109375000001E-2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>2.3491</v>
+      </c>
+      <c r="D10">
+        <v>54.4893</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>5.321220703125E-2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>2.3290000000000002</v>
+      </c>
+      <c r="I10">
+        <v>54.958399999999997</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>5.3670312499999998E-2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>256</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>2.3683999999999998</v>
+      </c>
+      <c r="D11">
+        <v>108.08969999999999</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.10555634765624999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <v>2.3694000000000002</v>
+      </c>
+      <c r="I11">
+        <v>108.0459</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0.10551357421875</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>512</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>2.4127000000000001</v>
+      </c>
+      <c r="D12">
+        <v>212.20910000000001</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.20723544921875001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12">
+        <v>2.3721000000000001</v>
+      </c>
+      <c r="I12">
+        <v>215.8424</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0.21078359375</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1024</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>2.5836000000000001</v>
+      </c>
+      <c r="D13">
+        <v>396.34890000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.38705947265625001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <v>2.5697999999999999</v>
+      </c>
+      <c r="I13">
+        <v>398.4794</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0.3891400390625</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2048</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>2.734</v>
+      </c>
+      <c r="D14">
+        <v>749.08309999999994</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.73152646484374995</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14">
+        <v>2.7635999999999998</v>
+      </c>
+      <c r="I14">
+        <v>741.06730000000005</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0.72369853515625004</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4096</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>8.0175999999999998</v>
+      </c>
+      <c r="D15">
+        <v>510.87869999999998</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.49890498046874998</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15">
+        <v>6.319</v>
+      </c>
+      <c r="I15">
+        <v>648.20719999999994</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0.63301484374999994</v>
+      </c>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8192</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>7.5484999999999998</v>
+      </c>
+      <c r="D16">
+        <v>1085.2552000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.0598195312500001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16">
+        <v>5.6883999999999997</v>
+      </c>
+      <c r="I16">
+        <v>1440.1158</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>1.4063630859375</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16384</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>7.8254000000000001</v>
+      </c>
+      <c r="D17">
+        <v>2093.7006999999999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2.0446295898437499</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17">
+        <v>5.7342000000000004</v>
+      </c>
+      <c r="I17">
+        <v>2857.2478999999998</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>2.7902811523437498</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>32768</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>8.2805999999999997</v>
+      </c>
+      <c r="D18">
+        <v>3957.1786000000002</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>3.8644322265625002</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>5.7061999999999999</v>
+      </c>
+      <c r="I18">
+        <v>5742.5424999999996</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>5.6079516601562496</v>
+      </c>
+      <c r="K18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>65536</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>9.4925999999999995</v>
+      </c>
+      <c r="D19">
+        <v>6903.8827000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>6.7420729492187501</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19">
+        <v>5.7736999999999998</v>
+      </c>
+      <c r="I19">
+        <v>11350.7971</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>11.08476279296875</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>131072</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>12.504099999999999</v>
+      </c>
+      <c r="D20">
+        <v>10482.3444</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>10.236664453125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20">
+        <v>8.9802999999999997</v>
+      </c>
+      <c r="I20">
+        <v>14595.494000000001</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>14.253412109375001</v>
+      </c>
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>262144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>19.102900000000002</v>
+      </c>
+      <c r="D21">
+        <v>13722.7073</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>13.40108134765625</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21">
+        <v>17.748799999999999</v>
+      </c>
+      <c r="I21">
+        <v>14769.6482</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>14.4234845703125</v>
+      </c>
+      <c r="K21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>524288</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>38.085999999999999</v>
+      </c>
+      <c r="D22">
+        <v>13765.9131</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>13.44327451171875</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>35.567999999999998</v>
+      </c>
+      <c r="I22">
+        <v>14740.4319</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>14.39495302734375</v>
+      </c>
+      <c r="K22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1048576</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>75.979200000000006</v>
+      </c>
+      <c r="D23">
+        <v>13800.8289</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>13.47737197265625</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23">
+        <v>71.798900000000003</v>
+      </c>
+      <c r="I23">
+        <v>14604.3472</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>14.2620578125</v>
+      </c>
+      <c r="K23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2097152</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>199.86009999999999</v>
+      </c>
+      <c r="D24">
+        <v>10493.100899999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>10.247168847656249</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24">
+        <v>150.7388</v>
+      </c>
+      <c r="I24">
+        <v>13912.4854</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>13.5864115234375</v>
+      </c>
+      <c r="K24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4194304</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>401.40800000000002</v>
+      </c>
+      <c r="D25">
+        <v>10448.9792</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>10.20408125</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25">
+        <v>309.24459999999999</v>
+      </c>
+      <c r="I25">
+        <v>13563.063200000001</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>13.24517890625</v>
+      </c>
+      <c r="K25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Merged review changes from hartmut
</commit_message>
<xml_diff>
--- a/2017-AC/serialization.xlsx
+++ b/2017-AC/serialization.xlsx
@@ -308,11 +308,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="206259712"/>
-        <c:axId val="674775616"/>
+        <c:axId val="670379520"/>
+        <c:axId val="675299904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="206259712"/>
+        <c:axId val="670379520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,7 +321,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674775616"/>
+        <c:crossAx val="675299904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -329,7 +329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="674775616"/>
+        <c:axId val="675299904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,7 +350,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206259712"/>
+        <c:crossAx val="670379520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -521,11 +521,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="668893184"/>
-        <c:axId val="674777344"/>
+        <c:axId val="670790144"/>
+        <c:axId val="675301632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="668893184"/>
+        <c:axId val="670790144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674777344"/>
+        <c:crossAx val="675301632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -542,7 +542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="674777344"/>
+        <c:axId val="675301632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="668893184"/>
+        <c:crossAx val="670790144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,11 +1159,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="674782528"/>
-        <c:axId val="669532160"/>
+        <c:axId val="675306816"/>
+        <c:axId val="671432704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="674782528"/>
+        <c:axId val="675306816"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1195,12 +1195,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="669532160"/>
+        <c:crossAx val="671432704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="669532160"/>
+        <c:axId val="671432704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,7 +1230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674782528"/>
+        <c:crossAx val="675306816"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1705,6 +1705,20 @@
           <c:marker>
             <c:symbol val="triangle"/>
             <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1872,11 +1886,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="669536768"/>
-        <c:axId val="669537344"/>
+        <c:axId val="671437312"/>
+        <c:axId val="671437888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="669536768"/>
+        <c:axId val="671437312"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1908,12 +1922,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="669537344"/>
+        <c:crossAx val="671437888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="669537344"/>
+        <c:axId val="671437888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +1957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="669536768"/>
+        <c:crossAx val="671437312"/>
         <c:crossesAt val="1.0000000000000004E-6"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2787,7 +2801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -4638,7 +4652,7 @@
         <v>0.3402</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:I50" si="6">H29/1024</f>
+        <f t="shared" ref="I29:I49" si="6">H29/1024</f>
         <v>3.322265625E-4</v>
       </c>
       <c r="J29" t="s">

</xml_diff>

<commit_message>
Fix axes on graph from s to us
</commit_message>
<xml_diff>
--- a/2017-AC/serialization.xlsx
+++ b/2017-AC/serialization.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="35">
   <si>
     <t>=</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>hpx_zero_copy</t>
+  </si>
+  <si>
+    <t>Time (us)</t>
+  </si>
+  <si>
+    <t>Iterations</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BEF59E7-ACFE-46EC-9BFB-22D5A022158A}" type="CELLRANGE">
+                    <a:fld id="{47CF54FC-4551-48C0-AC7E-FC787AFF901E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1112,7 +1118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{357FB4EA-05DD-4E69-8221-690CEC29F35F}" type="CELLRANGE">
+                    <a:fld id="{51BD4A90-A4A2-4DE2-B0AF-81186B84EAA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1147,7 +1153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19E1155A-9E21-4423-BE73-D06412C3FD59}" type="CELLRANGE">
+                    <a:fld id="{CF5689DB-8970-499C-B14C-F1E74197F874}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1183,7 +1189,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85B7B14D-BA54-4062-94A5-F28007B60781}" type="CELLRANGE">
+                    <a:fld id="{785ACD3F-C740-4CFA-9433-8717A4CB68F7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1224,7 +1230,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3440A737-CB0F-44A3-8978-74BF54F141EE}" type="CELLRANGE">
+                    <a:fld id="{7A739ECC-F178-4C33-82E2-2241E9CAE2A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1259,7 +1265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD5D35A3-359D-49CE-8F14-611244E0CA93}" type="CELLRANGE">
+                    <a:fld id="{CA42F08C-2ABB-4AC1-8013-4D6702C55CDC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1300,7 +1306,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D150CF0A-63D5-48EE-AFEA-47F7D474BA81}" type="CELLRANGE">
+                    <a:fld id="{A1D64597-757B-4648-BC13-33742A834383}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1335,7 +1341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4789B3F8-7892-465D-852A-89F2B5CF77C4}" type="CELLRANGE">
+                    <a:fld id="{9CCFC39D-67F7-49AA-BFC7-55B7CFAE5D75}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1467,7 +1473,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{135B2BA9-FB42-4BFA-B33B-3C79F651B433}" type="CELLRANGE">
+                    <a:fld id="{BB7510A3-457D-4112-A7A2-4A589502B5DE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -1531,7 +1537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1F676D8-D679-448F-96D7-521F561E3588}" type="CELLRANGE">
+                    <a:fld id="{814AA491-AAAE-42D1-8D65-606336203F55}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1572,7 +1578,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF985F87-B2E1-47F0-8176-8585333CBB20}" type="CELLRANGE">
+                    <a:fld id="{A716C18B-38A1-48FC-91D3-F2409749E808}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1612,7 +1618,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEB0B8BF-DF08-4AE5-8662-9D33D4F91D88}" type="CELLRANGE">
+                    <a:fld id="{F1C58D2B-0B6A-4872-9E85-0D6FBDF2C5DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1698,55 +1704,55 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'cpp-serializers'!$P$2:$P$14</c:f>
+              <c:f>'cpp-serializers'!$Q$2:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>14491</c:v>
+                  <c:v>14.491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22790</c:v>
+                  <c:v>22.79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16316</c:v>
+                  <c:v>16.315999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8222</c:v>
+                  <c:v>8.2219999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27203</c:v>
+                  <c:v>27.202999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6843</c:v>
+                  <c:v>6.843</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24010</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5798</c:v>
+                  <c:v>5.798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4164</c:v>
+                  <c:v>4.1639999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8838</c:v>
+                  <c:v>8.8379999999999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6019</c:v>
+                  <c:v>6.0190000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9603</c:v>
+                  <c:v>9.6029999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'cpp-serializers'!$V$2:$V$14</c:f>
+              <c:f>'cpp-serializers'!$W$2:$W$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1899,7 +1905,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Time taken to generate archive (ms)</a:t>
+                  <a:t>Time taken to generate archive (µs)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3637,16 +3643,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4022,10 +4028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="Q2" sqref="Q2:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4033,7 +4039,7 @@
     <col min="1" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4043,14 +4049,23 @@
       <c r="H1" t="s">
         <v>18</v>
       </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1">
+        <v>1000000</v>
+      </c>
       <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4087,26 +4102,30 @@
       <c r="P2">
         <v>14491</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2">
+        <f>1000*P2/K$1</f>
+        <v>14.491</v>
+      </c>
+      <c r="R2" t="s">
         <v>31</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>1</v>
       </c>
-      <c r="U2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2">
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>17017</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4143,26 +4162,30 @@
       <c r="P3">
         <v>22790</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q14" si="0">1000*P3/K$1</f>
+        <v>22.79</v>
+      </c>
+      <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>4</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>1</v>
       </c>
-      <c r="U3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3">
         <v>11597</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4199,26 +4222,30 @@
       <c r="P4">
         <v>16316</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>16.315999999999999</v>
+      </c>
+      <c r="R4" t="s">
         <v>31</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>5</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>1</v>
       </c>
-      <c r="U4" t="s">
-        <v>0</v>
-      </c>
-      <c r="V4">
+      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <v>12571</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -4255,26 +4282,30 @@
       <c r="P5">
         <v>31</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>3.1E-2</v>
+      </c>
+      <c r="R5" t="s">
         <v>31</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>6</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>1</v>
       </c>
-      <c r="U5" t="s">
-        <v>0</v>
-      </c>
-      <c r="V5">
+      <c r="V5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>17768</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4311,26 +4342,30 @@
       <c r="P6">
         <v>8222</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>8.2219999999999995</v>
+      </c>
+      <c r="R6" t="s">
         <v>31</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>7</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>1</v>
       </c>
-      <c r="U6" t="s">
-        <v>0</v>
-      </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>17470</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4367,26 +4402,30 @@
       <c r="P7">
         <v>27203</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>27.202999999999999</v>
+      </c>
+      <c r="R7" t="s">
         <v>31</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>8</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>1</v>
       </c>
-      <c r="U7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7">
         <v>11802</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4423,26 +4462,30 @@
       <c r="P8">
         <v>6843</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>6.843</v>
+      </c>
+      <c r="R8" t="s">
         <v>31</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>9</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>1</v>
       </c>
-      <c r="U8" t="s">
-        <v>0</v>
-      </c>
-      <c r="V8">
+      <c r="V8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>17416</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4479,26 +4522,30 @@
       <c r="P9">
         <v>24010</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>24.01</v>
+      </c>
+      <c r="R9" t="s">
         <v>31</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>10</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>1</v>
       </c>
-      <c r="U9" t="s">
-        <v>0</v>
-      </c>
-      <c r="V9">
+      <c r="V9" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>12288</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4535,26 +4582,30 @@
       <c r="P10">
         <v>5798</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>5.798</v>
+      </c>
+      <c r="R10" t="s">
         <v>31</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>11</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>1</v>
       </c>
-      <c r="U10" t="s">
-        <v>0</v>
-      </c>
-      <c r="V10">
+      <c r="V10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>17433</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4591,26 +4642,30 @@
       <c r="P11">
         <v>4164</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>4.1639999999999997</v>
+      </c>
+      <c r="R11" t="s">
         <v>31</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>32</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>1</v>
       </c>
-      <c r="U11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V11">
+      <c r="V11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11">
         <v>9433</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4647,26 +4702,30 @@
       <c r="P12">
         <v>8838</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>8.8379999999999992</v>
+      </c>
+      <c r="R12" t="s">
         <v>31</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>12</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>1</v>
       </c>
-      <c r="U12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12">
+      <c r="V12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <v>13008</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4703,26 +4762,30 @@
       <c r="P13">
         <v>6019</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>6.0190000000000001</v>
+      </c>
+      <c r="R13" t="s">
         <v>31</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>13</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>1</v>
       </c>
-      <c r="U13" t="s">
-        <v>0</v>
-      </c>
-      <c r="V13">
+      <c r="V13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>17423</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -4759,22 +4822,26 @@
       <c r="P14">
         <v>9603</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>9.6029999999999998</v>
+      </c>
+      <c r="R14" t="s">
         <v>31</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>14</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>1</v>
       </c>
-      <c r="U14" t="s">
-        <v>0</v>
-      </c>
-      <c r="V14">
+      <c r="V14" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14">
         <v>17632</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>